<commit_message>
See, it was not finished yet
</commit_message>
<xml_diff>
--- a/output/sites/clustering with PCs/clust_PCs_compo_sites.xlsx
+++ b/output/sites/clustering with PCs/clust_PCs_compo_sites.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t xml:space="preserve">site</t>
   </si>
@@ -20,40 +20,58 @@
     <t xml:space="preserve">cluster</t>
   </si>
   <si>
+    <t xml:space="preserve">median_Fe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">median_Zn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">median_Cu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">median_Mn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">median_Se</t>
+  </si>
+  <si>
+    <t xml:space="preserve">median_Co</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mean_Fe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mean_Zn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mean_Cu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mean_Mn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mean_Se</t>
+  </si>
+  <si>
     <t xml:space="preserve">mean_Co</t>
   </si>
   <si>
-    <t xml:space="preserve">mean_Cu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mean_Fe</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mean_Mn</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mean_Se</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mean_Zn</t>
+    <t xml:space="preserve">sd_Fe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sd_Zn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sd_Cu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sd_Mn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sd_Se</t>
   </si>
   <si>
     <t xml:space="preserve">sd_Co</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sd_Cu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sd_Fe</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sd_Mn</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sd_Se</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sd_Zn</t>
   </si>
   <si>
     <t xml:space="preserve">Cap Noir</t>
@@ -434,357 +452,519 @@
       <c r="N1" t="s">
         <v>13</v>
       </c>
+      <c r="O1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="B2" t="n">
         <v>1</v>
       </c>
       <c r="C2" t="n">
+        <v>316.983</v>
+      </c>
+      <c r="D2" t="n">
+        <v>435.684</v>
+      </c>
+      <c r="E2" t="n">
+        <v>46.899</v>
+      </c>
+      <c r="F2" t="n">
+        <v>22.098</v>
+      </c>
+      <c r="G2" t="n">
+        <v>9.208</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0.189</v>
+      </c>
+      <c r="I2" t="n">
+        <v>262.874</v>
+      </c>
+      <c r="J2" t="n">
+        <v>542.414</v>
+      </c>
+      <c r="K2" t="n">
+        <v>72.246</v>
+      </c>
+      <c r="L2" t="n">
+        <v>20.704</v>
+      </c>
+      <c r="M2" t="n">
+        <v>11.346</v>
+      </c>
+      <c r="N2" t="n">
         <v>0.323</v>
       </c>
-      <c r="D2" t="n">
-        <v>72.246</v>
-      </c>
-      <c r="E2" t="n">
-        <v>262.874</v>
-      </c>
-      <c r="F2" t="n">
-        <v>20.704</v>
-      </c>
-      <c r="G2" t="n">
-        <v>11.346</v>
-      </c>
-      <c r="H2" t="n">
-        <v>542.414</v>
-      </c>
-      <c r="I2" t="n">
+      <c r="O2" t="n">
+        <v>80.398</v>
+      </c>
+      <c r="P2" t="n">
+        <v>313.417</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>77.19</v>
+      </c>
+      <c r="R2" t="n">
+        <v>2.414</v>
+      </c>
+      <c r="S2" t="n">
+        <v>7.698</v>
+      </c>
+      <c r="T2" t="n">
         <v>0.241</v>
-      </c>
-      <c r="J2" t="n">
-        <v>77.19</v>
-      </c>
-      <c r="K2" t="n">
-        <v>80.398</v>
-      </c>
-      <c r="L2" t="n">
-        <v>2.414</v>
-      </c>
-      <c r="M2" t="n">
-        <v>7.698</v>
-      </c>
-      <c r="N2" t="n">
-        <v>313.417</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="B3" t="n">
         <v>2</v>
       </c>
       <c r="C3" t="n">
+        <v>8194.809</v>
+      </c>
+      <c r="D3" t="n">
+        <v>542.588</v>
+      </c>
+      <c r="E3" t="n">
+        <v>227.139</v>
+      </c>
+      <c r="F3" t="n">
+        <v>142.476</v>
+      </c>
+      <c r="G3" t="n">
+        <v>24.59</v>
+      </c>
+      <c r="H3" t="n">
+        <v>6.608</v>
+      </c>
+      <c r="I3" t="n">
+        <v>9143.862</v>
+      </c>
+      <c r="J3" t="n">
+        <v>481.124</v>
+      </c>
+      <c r="K3" t="n">
+        <v>300.064</v>
+      </c>
+      <c r="L3" t="n">
+        <v>130.531</v>
+      </c>
+      <c r="M3" t="n">
+        <v>30.356</v>
+      </c>
+      <c r="N3" t="n">
         <v>7.033</v>
       </c>
-      <c r="D3" t="n">
-        <v>300.064</v>
-      </c>
-      <c r="E3" t="n">
-        <v>9143.862</v>
-      </c>
-      <c r="F3" t="n">
-        <v>130.531</v>
-      </c>
-      <c r="G3" t="n">
-        <v>30.356</v>
-      </c>
-      <c r="H3" t="n">
-        <v>481.124</v>
-      </c>
-      <c r="I3" t="n">
+      <c r="O3" t="n">
+        <v>4214.898</v>
+      </c>
+      <c r="P3" t="n">
+        <v>186.88</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>235.323</v>
+      </c>
+      <c r="R3" t="n">
+        <v>49.482</v>
+      </c>
+      <c r="S3" t="n">
+        <v>11.082</v>
+      </c>
+      <c r="T3" t="n">
         <v>3.161</v>
-      </c>
-      <c r="J3" t="n">
-        <v>235.323</v>
-      </c>
-      <c r="K3" t="n">
-        <v>4214.898</v>
-      </c>
-      <c r="L3" t="n">
-        <v>49.482</v>
-      </c>
-      <c r="M3" t="n">
-        <v>11.082</v>
-      </c>
-      <c r="N3" t="n">
-        <v>186.88</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="B4" t="n">
         <v>3</v>
       </c>
       <c r="C4" t="n">
+        <v>2128.066</v>
+      </c>
+      <c r="D4" t="n">
+        <v>566.289</v>
+      </c>
+      <c r="E4" t="n">
+        <v>235.579</v>
+      </c>
+      <c r="F4" t="n">
+        <v>51.078</v>
+      </c>
+      <c r="G4" t="n">
+        <v>43.147</v>
+      </c>
+      <c r="H4" t="n">
+        <v>1.798</v>
+      </c>
+      <c r="I4" t="n">
+        <v>2068.141</v>
+      </c>
+      <c r="J4" t="n">
+        <v>573.772</v>
+      </c>
+      <c r="K4" t="n">
+        <v>297.74</v>
+      </c>
+      <c r="L4" t="n">
+        <v>70.775</v>
+      </c>
+      <c r="M4" t="n">
+        <v>40.061</v>
+      </c>
+      <c r="N4" t="n">
         <v>1.971</v>
       </c>
-      <c r="D4" t="n">
-        <v>297.74</v>
-      </c>
-      <c r="E4" t="n">
-        <v>2068.141</v>
-      </c>
-      <c r="F4" t="n">
-        <v>70.775</v>
-      </c>
-      <c r="G4" t="n">
-        <v>40.061</v>
-      </c>
-      <c r="H4" t="n">
-        <v>573.772</v>
-      </c>
-      <c r="I4" t="n">
+      <c r="O4" t="n">
+        <v>658.644</v>
+      </c>
+      <c r="P4" t="n">
+        <v>205.022</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>199.305</v>
+      </c>
+      <c r="R4" t="n">
+        <v>45.196</v>
+      </c>
+      <c r="S4" t="n">
+        <v>21.113</v>
+      </c>
+      <c r="T4" t="n">
         <v>1.157</v>
-      </c>
-      <c r="J4" t="n">
-        <v>199.305</v>
-      </c>
-      <c r="K4" t="n">
-        <v>658.644</v>
-      </c>
-      <c r="L4" t="n">
-        <v>45.196</v>
-      </c>
-      <c r="M4" t="n">
-        <v>21.113</v>
-      </c>
-      <c r="N4" t="n">
-        <v>205.022</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="B5" t="n">
         <v>4</v>
       </c>
       <c r="C5" t="n">
+        <v>233.248</v>
+      </c>
+      <c r="D5" t="n">
+        <v>105.864</v>
+      </c>
+      <c r="E5" t="n">
+        <v>346.17</v>
+      </c>
+      <c r="F5" t="n">
+        <v>16.106</v>
+      </c>
+      <c r="G5" t="n">
+        <v>85.952</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0.252</v>
+      </c>
+      <c r="I5" t="n">
+        <v>215.956</v>
+      </c>
+      <c r="J5" t="n">
+        <v>180.555</v>
+      </c>
+      <c r="K5" t="n">
+        <v>415.994</v>
+      </c>
+      <c r="L5" t="n">
+        <v>15.795</v>
+      </c>
+      <c r="M5" t="n">
+        <v>88.946</v>
+      </c>
+      <c r="N5" t="n">
         <v>0.348</v>
       </c>
-      <c r="D5" t="n">
-        <v>415.994</v>
-      </c>
-      <c r="E5" t="n">
-        <v>215.956</v>
-      </c>
-      <c r="F5" t="n">
-        <v>15.795</v>
-      </c>
-      <c r="G5" t="n">
-        <v>88.946</v>
-      </c>
-      <c r="H5" t="n">
-        <v>180.555</v>
-      </c>
-      <c r="I5" t="n">
+      <c r="O5" t="n">
+        <v>45.723</v>
+      </c>
+      <c r="P5" t="n">
+        <v>169.632</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>203.898</v>
+      </c>
+      <c r="R5" t="n">
+        <v>2.357</v>
+      </c>
+      <c r="S5" t="n">
+        <v>31.916</v>
+      </c>
+      <c r="T5" t="n">
         <v>0.281</v>
-      </c>
-      <c r="J5" t="n">
-        <v>203.898</v>
-      </c>
-      <c r="K5" t="n">
-        <v>45.723</v>
-      </c>
-      <c r="L5" t="n">
-        <v>2.357</v>
-      </c>
-      <c r="M5" t="n">
-        <v>31.916</v>
-      </c>
-      <c r="N5" t="n">
-        <v>169.632</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="B6" t="n">
         <v>1</v>
       </c>
       <c r="C6" t="n">
+        <v>310.797</v>
+      </c>
+      <c r="D6" t="n">
+        <v>279.906</v>
+      </c>
+      <c r="E6" t="n">
+        <v>19.797</v>
+      </c>
+      <c r="F6" t="n">
+        <v>18.059</v>
+      </c>
+      <c r="G6" t="n">
+        <v>7.634</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0.513</v>
+      </c>
+      <c r="I6" t="n">
+        <v>380.912</v>
+      </c>
+      <c r="J6" t="n">
+        <v>319.393</v>
+      </c>
+      <c r="K6" t="n">
+        <v>32.334</v>
+      </c>
+      <c r="L6" t="n">
+        <v>19.921</v>
+      </c>
+      <c r="M6" t="n">
+        <v>9.973</v>
+      </c>
+      <c r="N6" t="n">
         <v>0.57</v>
       </c>
-      <c r="D6" t="n">
-        <v>32.334</v>
-      </c>
-      <c r="E6" t="n">
-        <v>380.912</v>
-      </c>
-      <c r="F6" t="n">
-        <v>19.921</v>
-      </c>
-      <c r="G6" t="n">
-        <v>9.973</v>
-      </c>
-      <c r="H6" t="n">
-        <v>319.393</v>
-      </c>
-      <c r="I6" t="n">
+      <c r="O6" t="n">
+        <v>216.797</v>
+      </c>
+      <c r="P6" t="n">
+        <v>88.688</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>23.942</v>
+      </c>
+      <c r="R6" t="n">
+        <v>5.714</v>
+      </c>
+      <c r="S6" t="n">
+        <v>5.809</v>
+      </c>
+      <c r="T6" t="n">
         <v>0.245</v>
-      </c>
-      <c r="J6" t="n">
-        <v>23.942</v>
-      </c>
-      <c r="K6" t="n">
-        <v>216.797</v>
-      </c>
-      <c r="L6" t="n">
-        <v>5.714</v>
-      </c>
-      <c r="M6" t="n">
-        <v>5.809</v>
-      </c>
-      <c r="N6" t="n">
-        <v>88.688</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="B7" t="n">
         <v>2</v>
       </c>
       <c r="C7" t="n">
+        <v>7299.135</v>
+      </c>
+      <c r="D7" t="n">
+        <v>597.222</v>
+      </c>
+      <c r="E7" t="n">
+        <v>160.849</v>
+      </c>
+      <c r="F7" t="n">
+        <v>130.412</v>
+      </c>
+      <c r="G7" t="n">
+        <v>32.234</v>
+      </c>
+      <c r="H7" t="n">
+        <v>6.774</v>
+      </c>
+      <c r="I7" t="n">
+        <v>6147.18</v>
+      </c>
+      <c r="J7" t="n">
+        <v>499.664</v>
+      </c>
+      <c r="K7" t="n">
+        <v>163.777</v>
+      </c>
+      <c r="L7" t="n">
+        <v>151.869</v>
+      </c>
+      <c r="M7" t="n">
+        <v>27.418</v>
+      </c>
+      <c r="N7" t="n">
         <v>5.268</v>
       </c>
-      <c r="D7" t="n">
-        <v>163.777</v>
-      </c>
-      <c r="E7" t="n">
-        <v>6147.18</v>
-      </c>
-      <c r="F7" t="n">
-        <v>151.869</v>
-      </c>
-      <c r="G7" t="n">
-        <v>27.418</v>
-      </c>
-      <c r="H7" t="n">
-        <v>499.664</v>
-      </c>
-      <c r="I7" t="n">
+      <c r="O7" t="n">
+        <v>4000.33</v>
+      </c>
+      <c r="P7" t="n">
+        <v>297.229</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>124.458</v>
+      </c>
+      <c r="R7" t="n">
+        <v>117.391</v>
+      </c>
+      <c r="S7" t="n">
+        <v>14.5</v>
+      </c>
+      <c r="T7" t="n">
         <v>3.887</v>
-      </c>
-      <c r="J7" t="n">
-        <v>124.458</v>
-      </c>
-      <c r="K7" t="n">
-        <v>4000.33</v>
-      </c>
-      <c r="L7" t="n">
-        <v>117.391</v>
-      </c>
-      <c r="M7" t="n">
-        <v>14.5</v>
-      </c>
-      <c r="N7" t="n">
-        <v>297.229</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="B8" t="n">
         <v>3</v>
       </c>
       <c r="C8" t="n">
+        <v>212.54</v>
+      </c>
+      <c r="D8" t="n">
+        <v>332.478</v>
+      </c>
+      <c r="E8" t="n">
+        <v>59.187</v>
+      </c>
+      <c r="F8" t="n">
+        <v>19.678</v>
+      </c>
+      <c r="G8" t="n">
+        <v>23.621</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0.373</v>
+      </c>
+      <c r="I8" t="n">
+        <v>257.886</v>
+      </c>
+      <c r="J8" t="n">
+        <v>263.916</v>
+      </c>
+      <c r="K8" t="n">
+        <v>69.598</v>
+      </c>
+      <c r="L8" t="n">
+        <v>18.425</v>
+      </c>
+      <c r="M8" t="n">
+        <v>25.23</v>
+      </c>
+      <c r="N8" t="n">
         <v>0.384</v>
       </c>
-      <c r="D8" t="n">
-        <v>69.598</v>
-      </c>
-      <c r="E8" t="n">
-        <v>257.886</v>
-      </c>
-      <c r="F8" t="n">
-        <v>18.425</v>
-      </c>
-      <c r="G8" t="n">
-        <v>25.23</v>
-      </c>
-      <c r="H8" t="n">
-        <v>263.916</v>
-      </c>
-      <c r="I8" t="n">
+      <c r="O8" t="n">
+        <v>181.958</v>
+      </c>
+      <c r="P8" t="n">
+        <v>164.644</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>40.011</v>
+      </c>
+      <c r="R8" t="n">
+        <v>4.549</v>
+      </c>
+      <c r="S8" t="n">
+        <v>12.359</v>
+      </c>
+      <c r="T8" t="n">
         <v>0.212</v>
-      </c>
-      <c r="J8" t="n">
-        <v>40.011</v>
-      </c>
-      <c r="K8" t="n">
-        <v>181.958</v>
-      </c>
-      <c r="L8" t="n">
-        <v>4.549</v>
-      </c>
-      <c r="M8" t="n">
-        <v>12.359</v>
-      </c>
-      <c r="N8" t="n">
-        <v>164.644</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="B9" t="n">
         <v>4</v>
       </c>
       <c r="C9" t="n">
+        <v>11288.645</v>
+      </c>
+      <c r="D9" t="n">
+        <v>249.605</v>
+      </c>
+      <c r="E9" t="n">
+        <v>214.971</v>
+      </c>
+      <c r="F9" t="n">
+        <v>266.478</v>
+      </c>
+      <c r="G9" t="n">
+        <v>50.094</v>
+      </c>
+      <c r="H9" t="n">
+        <v>6.326</v>
+      </c>
+      <c r="I9" t="n">
+        <v>9878.191</v>
+      </c>
+      <c r="J9" t="n">
+        <v>264.216</v>
+      </c>
+      <c r="K9" t="n">
+        <v>236.71</v>
+      </c>
+      <c r="L9" t="n">
+        <v>272.993</v>
+      </c>
+      <c r="M9" t="n">
+        <v>54.049</v>
+      </c>
+      <c r="N9" t="n">
         <v>6.486</v>
       </c>
-      <c r="D9" t="n">
-        <v>236.71</v>
-      </c>
-      <c r="E9" t="n">
-        <v>9878.191</v>
-      </c>
-      <c r="F9" t="n">
-        <v>272.993</v>
-      </c>
-      <c r="G9" t="n">
-        <v>54.049</v>
-      </c>
-      <c r="H9" t="n">
-        <v>264.216</v>
-      </c>
-      <c r="I9" t="n">
+      <c r="O9" t="n">
+        <v>4347.953</v>
+      </c>
+      <c r="P9" t="n">
+        <v>154.008</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>131.742</v>
+      </c>
+      <c r="R9" t="n">
+        <v>113.472</v>
+      </c>
+      <c r="S9" t="n">
+        <v>22.815</v>
+      </c>
+      <c r="T9" t="n">
         <v>1.38</v>
-      </c>
-      <c r="J9" t="n">
-        <v>131.742</v>
-      </c>
-      <c r="K9" t="n">
-        <v>4347.953</v>
-      </c>
-      <c r="L9" t="n">
-        <v>113.472</v>
-      </c>
-      <c r="M9" t="n">
-        <v>22.815</v>
-      </c>
-      <c r="N9" t="n">
-        <v>154.008</v>
       </c>
     </row>
   </sheetData>

</xml_diff>